<commit_message>
completed data extraction and data merge
</commit_message>
<xml_diff>
--- a/data/cleaned_data/2015_TN.xlsx
+++ b/data/cleaned_data/2015_TN.xlsx
@@ -1,26 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25225"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\iulia\Documents\NSS\projects\capstone\data\cleaned_data\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2299CD7-7BEB-4102-B74A-65B2F3F0A7F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="514" uniqueCount="333">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="518" uniqueCount="334">
   <si>
     <t>County</t>
   </si>
@@ -299,6 +293,9 @@
   </si>
   <si>
     <t>Union</t>
+  </si>
+  <si>
+    <t>Unknown</t>
   </si>
   <si>
     <t>VanBuren</t>
@@ -1024,8 +1021,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1088,14 +1085,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -1142,7 +1131,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1174,27 +1163,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1226,24 +1197,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1419,16 +1372,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G96"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:G97"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="N82" sqref="N82"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1451,1882 +1402,1873 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7">
       <c r="A2" t="s">
         <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C2" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="D2" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="E2">
         <v>75456</v>
       </c>
       <c r="F2" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="G2" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
       <c r="A3" t="s">
         <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C3" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="D3" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="E3">
         <v>46948</v>
       </c>
       <c r="F3" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="G3" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
       <c r="A4" t="s">
         <v>8</v>
       </c>
       <c r="B4" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C4" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="D4" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="E4">
         <v>16220</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7">
       <c r="A5" t="s">
         <v>9</v>
       </c>
       <c r="B5" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C5" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="D5" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="E5">
         <v>14601</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7">
       <c r="A6" t="s">
         <v>10</v>
       </c>
       <c r="B6" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C6" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="D6" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="E6">
         <v>126954</v>
       </c>
       <c r="F6" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="G6" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
       <c r="A7" t="s">
         <v>11</v>
       </c>
       <c r="B7" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C7" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="D7" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="E7">
         <v>103774</v>
       </c>
       <c r="F7" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="G7" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
       <c r="A8" t="s">
         <v>12</v>
       </c>
       <c r="B8" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C8" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="D8" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="E8">
         <v>39772</v>
       </c>
       <c r="F8" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="G8" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
       <c r="A9" t="s">
         <v>13</v>
       </c>
       <c r="B9" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C9" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="D9" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="E9">
         <v>13740</v>
       </c>
       <c r="F9" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="G9" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
       <c r="A10" t="s">
         <v>14</v>
       </c>
       <c r="B10" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C10" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="D10" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="E10">
         <v>27982</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7">
       <c r="A11" t="s">
         <v>15</v>
       </c>
       <c r="B11" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C11" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="D11" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="E11">
         <v>56375</v>
       </c>
       <c r="F11" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="G11" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
       <c r="A12" t="s">
         <v>16</v>
       </c>
       <c r="B12" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C12" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D12" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="E12">
         <v>39593</v>
       </c>
       <c r="F12" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="G12" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
       <c r="A13" t="s">
         <v>17</v>
       </c>
       <c r="B13" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C13" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="D13" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="E13">
         <v>17123</v>
       </c>
       <c r="F13" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="G13" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
       <c r="A14" t="s">
         <v>18</v>
       </c>
       <c r="B14" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C14" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="D14" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="E14">
         <v>31555</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7">
       <c r="A15" t="s">
         <v>19</v>
       </c>
       <c r="B15" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C15" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="D15" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="E15">
         <v>7663</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7">
       <c r="A16" t="s">
         <v>20</v>
       </c>
       <c r="B16" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C16" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="D16" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="E16">
         <v>35138</v>
       </c>
       <c r="F16" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="G16" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
       <c r="A17" t="s">
         <v>21</v>
       </c>
       <c r="B17" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C17" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="D17" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="E17">
         <v>54093</v>
       </c>
       <c r="F17" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="G17" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
       <c r="A18" t="s">
         <v>22</v>
       </c>
       <c r="B18" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C18" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="D18" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="E18">
         <v>14586</v>
       </c>
       <c r="F18" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="G18" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7">
       <c r="A19" t="s">
         <v>23</v>
       </c>
       <c r="B19" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C19" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="D19" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="E19">
         <v>58217</v>
       </c>
       <c r="F19" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="G19" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7">
       <c r="A20" t="s">
         <v>24</v>
       </c>
       <c r="B20" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="C20" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="D20" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="E20">
         <v>679793</v>
       </c>
       <c r="F20" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="G20" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7">
       <c r="A21" t="s">
         <v>25</v>
       </c>
       <c r="B21" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C21" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="D21" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="E21">
         <v>11600</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7">
       <c r="A22" t="s">
         <v>26</v>
       </c>
       <c r="B22" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C22" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="D22" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="E22">
         <v>19292</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7">
       <c r="A23" t="s">
         <v>27</v>
       </c>
       <c r="B23" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C23" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="D23" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="E23">
         <v>51334</v>
       </c>
       <c r="F23" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="G23" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7">
       <c r="A24" t="s">
         <v>28</v>
       </c>
       <c r="B24" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C24" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="D24" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="E24">
         <v>37753</v>
       </c>
       <c r="F24" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="G24" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7">
       <c r="A25" t="s">
         <v>29</v>
       </c>
       <c r="B25" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C25" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="D25" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="E25">
         <v>39280</v>
       </c>
       <c r="F25" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="G25" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7">
       <c r="A26" t="s">
         <v>30</v>
       </c>
       <c r="B26" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C26" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="D26" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="E26">
         <v>17965</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7">
       <c r="A27" t="s">
         <v>31</v>
       </c>
       <c r="B27" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C27" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="D27" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="E27">
         <v>41343</v>
       </c>
       <c r="F27" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="G27" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7">
       <c r="A28" t="s">
         <v>32</v>
       </c>
       <c r="B28" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C28" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="D28" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="E28">
         <v>49329</v>
       </c>
       <c r="F28" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="G28" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7">
       <c r="A29" t="s">
         <v>33</v>
       </c>
       <c r="B29" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C29" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="D29" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="E29">
         <v>28973</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7">
       <c r="A30" t="s">
         <v>34</v>
       </c>
       <c r="B30" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C30" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="D30" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="E30">
         <v>22848</v>
       </c>
       <c r="F30" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="G30" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7">
       <c r="A31" t="s">
         <v>35</v>
       </c>
       <c r="B31" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C31" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="D31" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="E31">
         <v>68586</v>
       </c>
       <c r="F31" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="G31" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7">
       <c r="A32" t="s">
         <v>36</v>
       </c>
       <c r="B32" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C32" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="D32" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="E32">
         <v>13337</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7">
       <c r="A33" t="s">
         <v>37</v>
       </c>
       <c r="B33" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C33" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="D33" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="E33">
         <v>63353</v>
       </c>
       <c r="F33" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="G33" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7">
       <c r="A34" t="s">
         <v>38</v>
       </c>
       <c r="B34" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C34" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="D34" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="E34">
         <v>353690</v>
       </c>
       <c r="F34" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="G34" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7">
       <c r="A35" t="s">
         <v>39</v>
       </c>
       <c r="B35" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C35" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="D35" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="E35">
         <v>6577</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7">
       <c r="A36" t="s">
         <v>40</v>
       </c>
       <c r="B36" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C36" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="D36" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="E36">
         <v>25817</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7">
       <c r="A37" t="s">
         <v>41</v>
       </c>
       <c r="B37" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C37" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="D37" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="E37">
         <v>25754</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7">
       <c r="A38" t="s">
         <v>42</v>
       </c>
       <c r="B38" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="C38" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="D38" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="E38">
         <v>56370</v>
       </c>
       <c r="F38" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="G38" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7">
       <c r="A39" t="s">
         <v>43</v>
       </c>
       <c r="B39" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C39" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="D39" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="E39">
         <v>18036</v>
       </c>
       <c r="F39" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="G39" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7">
       <c r="A40" t="s">
         <v>44</v>
       </c>
       <c r="B40" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="C40" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="D40" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="E40">
         <v>28078</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7">
       <c r="A41" t="s">
         <v>45</v>
       </c>
       <c r="B41" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="C41" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="D41" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="E41">
         <v>32127</v>
       </c>
       <c r="F41" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="G41" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7">
       <c r="A42" t="s">
         <v>46</v>
       </c>
       <c r="B42" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C42" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="D42" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="E42">
         <v>24373</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7">
       <c r="A43" t="s">
         <v>47</v>
       </c>
       <c r="B43" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C43" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="D43" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="E43">
         <v>8124</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7">
       <c r="A44" t="s">
         <v>48</v>
       </c>
       <c r="B44" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C44" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="D44" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="E44">
         <v>18157</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7">
       <c r="A45" t="s">
         <v>49</v>
       </c>
       <c r="B45" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C45" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="D45" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="E45">
         <v>11534</v>
       </c>
       <c r="F45" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="G45" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7">
       <c r="A46" t="s">
         <v>50</v>
       </c>
       <c r="B46" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C46" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="D46" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="E46">
         <v>53011</v>
       </c>
       <c r="F46" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="G46" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7">
       <c r="A47" t="s">
         <v>51</v>
       </c>
       <c r="B47" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C47" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="D47" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="E47">
         <v>17842</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7">
       <c r="A48" t="s">
         <v>52</v>
       </c>
       <c r="B48" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C48" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="D48" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="E48">
         <v>451297</v>
       </c>
       <c r="F48" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="G48" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7">
       <c r="A49" t="s">
         <v>53</v>
       </c>
       <c r="B49" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C49" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="D49" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="E49">
         <v>7602</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:7">
       <c r="A50" t="s">
         <v>54</v>
       </c>
       <c r="B50" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C50" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="D50" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="E50">
         <v>26903</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:7">
       <c r="A51" t="s">
         <v>55</v>
       </c>
       <c r="B51" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C51" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="D51" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="E51">
         <v>42592</v>
       </c>
       <c r="F51" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="G51" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7">
       <c r="A52" t="s">
         <v>56</v>
       </c>
       <c r="B52" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C52" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="D52" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="E52">
         <v>11875</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:7">
       <c r="A53" t="s">
         <v>57</v>
       </c>
       <c r="B53" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C53" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="D53" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="E53">
         <v>33609</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:7">
       <c r="A54" t="s">
         <v>58</v>
       </c>
       <c r="B54" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C54" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="D54" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="E54">
         <v>50916</v>
       </c>
       <c r="F54" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="G54" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7">
       <c r="A55" t="s">
         <v>59</v>
       </c>
       <c r="B55" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C55" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="D55" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="E55">
         <v>23076</v>
       </c>
       <c r="F55" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="G55" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7">
       <c r="A56" t="s">
         <v>60</v>
       </c>
       <c r="B56" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C56" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="D56" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="E56">
         <v>97569</v>
       </c>
       <c r="F56" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="G56" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7">
       <c r="A57" t="s">
         <v>61</v>
       </c>
       <c r="B57" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C57" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="D57" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="E57">
         <v>28397</v>
       </c>
       <c r="F57" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="G57" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7">
       <c r="A58" t="s">
         <v>62</v>
       </c>
       <c r="B58" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C58" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="D58" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="E58">
         <v>31590</v>
       </c>
       <c r="F58" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="G58" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7">
       <c r="A59" t="s">
         <v>63</v>
       </c>
       <c r="B59" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C59" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="D59" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="E59">
         <v>87425</v>
       </c>
       <c r="F59" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="G59" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7">
       <c r="A60" t="s">
         <v>64</v>
       </c>
       <c r="B60" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C60" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="D60" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="E60">
         <v>52502</v>
       </c>
       <c r="F60" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="G60" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7">
       <c r="A61" t="s">
         <v>65</v>
       </c>
       <c r="B61" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C61" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="D61" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="E61">
         <v>25864</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:7">
       <c r="A62" t="s">
         <v>66</v>
       </c>
       <c r="B62" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C62" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="D62" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="E62">
         <v>11804</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:7">
       <c r="A63" t="s">
         <v>67</v>
       </c>
       <c r="B63" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C63" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="D63" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="E63">
         <v>45625</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:7">
       <c r="A64" t="s">
         <v>68</v>
       </c>
       <c r="B64" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C64" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="D64" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="E64">
         <v>192398</v>
       </c>
       <c r="F64" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="G64" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7">
       <c r="A65" t="s">
         <v>69</v>
       </c>
       <c r="B65" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C65" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="D65" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="E65">
         <v>6261</v>
       </c>
       <c r="F65" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="G65" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7">
       <c r="A66" t="s">
         <v>70</v>
       </c>
       <c r="B66" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C66" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="D66" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="E66">
         <v>21494</v>
       </c>
       <c r="F66" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="G66" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7">
       <c r="A67" t="s">
         <v>71</v>
       </c>
       <c r="B67" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C67" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="D67" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="E67">
         <v>30561</v>
       </c>
       <c r="F67" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="G67" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7">
       <c r="A68" t="s">
         <v>72</v>
       </c>
       <c r="B68" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C68" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="D68" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="E68">
         <v>22067</v>
       </c>
       <c r="F68" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="G68" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7">
       <c r="A69" t="s">
         <v>73</v>
       </c>
       <c r="B69" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C69" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="D69" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="E69">
         <v>7852</v>
       </c>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:7">
       <c r="A70" t="s">
         <v>74</v>
       </c>
       <c r="B70" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C70" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="D70" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="E70">
         <v>5139</v>
       </c>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:7">
       <c r="A71" t="s">
         <v>75</v>
       </c>
       <c r="B71" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C71" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="D71" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="E71">
         <v>16769</v>
       </c>
       <c r="F71" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="G71" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7">
       <c r="A72" t="s">
         <v>76</v>
       </c>
       <c r="B72" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C72" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="D72" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="E72">
         <v>75074</v>
       </c>
       <c r="F72" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="G72" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7">
       <c r="A73" t="s">
         <v>77</v>
       </c>
       <c r="B73" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="C73" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="D73" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="E73">
         <v>32373</v>
       </c>
       <c r="F73" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="G73" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7">
       <c r="A74" t="s">
         <v>78</v>
       </c>
       <c r="B74" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C74" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="D74" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="E74">
         <v>52770</v>
       </c>
       <c r="F74" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="G74" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7">
       <c r="A75" t="s">
         <v>79</v>
       </c>
       <c r="B75" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C75" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="D75" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="E75">
         <v>68687</v>
       </c>
       <c r="F75" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="G75" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7">
       <c r="A76" t="s">
         <v>80</v>
       </c>
       <c r="B76" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C76" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="D76" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="E76">
         <v>298197</v>
       </c>
       <c r="F76" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="G76" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7">
       <c r="A77" t="s">
         <v>81</v>
       </c>
       <c r="B77" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C77" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="D77" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="E77">
         <v>21893</v>
       </c>
     </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:7">
       <c r="A78" t="s">
         <v>82</v>
       </c>
       <c r="B78" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C78" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="D78" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="E78">
         <v>14641</v>
       </c>
       <c r="F78" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="G78" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7">
       <c r="A79" t="s">
         <v>83</v>
       </c>
       <c r="B79" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C79" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="D79" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="E79">
         <v>95417</v>
       </c>
       <c r="F79" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="G79" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7">
       <c r="A80" t="s">
         <v>84</v>
       </c>
       <c r="B80" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C80" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="D80" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="E80">
         <v>937067</v>
       </c>
       <c r="F80" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="G80" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7">
       <c r="A81" t="s">
         <v>85</v>
       </c>
       <c r="B81" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C81" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="D81" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="E81">
         <v>19308</v>
       </c>
       <c r="F81" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="G81" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7">
       <c r="A82" t="s">
         <v>86</v>
       </c>
       <c r="B82" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C82" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="D82" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="E82">
         <v>13187</v>
       </c>
       <c r="F82" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="G82" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7">
       <c r="A83" t="s">
         <v>87</v>
       </c>
       <c r="B83" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C83" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="D83" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="E83">
         <v>156199</v>
       </c>
       <c r="F83" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="G83" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7">
       <c r="A84" t="s">
         <v>88</v>
       </c>
       <c r="B84" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C84" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="D84" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="E84">
         <v>175326</v>
       </c>
       <c r="F84" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="G84" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7">
       <c r="A85" t="s">
         <v>89</v>
       </c>
       <c r="B85" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C85" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="D85" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="E85">
         <v>61533</v>
       </c>
       <c r="F85" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="G85" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7">
       <c r="A86" t="s">
         <v>90</v>
       </c>
       <c r="B86" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C86" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="D86" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="E86">
         <v>8051</v>
       </c>
       <c r="F86" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="G86" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7">
       <c r="A87" t="s">
         <v>91</v>
       </c>
       <c r="B87" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C87" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="D87" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="E87">
         <v>17819</v>
       </c>
       <c r="F87" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="G87" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7">
       <c r="A88" t="s">
         <v>92</v>
       </c>
       <c r="B88" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C88" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="D88" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="E88">
         <v>19159</v>
       </c>
       <c r="F88" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="G88" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7">
       <c r="A89" t="s">
         <v>93</v>
       </c>
       <c r="B89" t="s">
-        <v>104</v>
+        <v>118</v>
       </c>
       <c r="C89" t="s">
-        <v>206</v>
+        <v>118</v>
       </c>
       <c r="D89" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7">
       <c r="A90" t="s">
         <v>94</v>
       </c>
       <c r="B90" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="C90" t="s">
         <v>207</v>
       </c>
       <c r="D90" t="s">
-        <v>297</v>
-      </c>
-      <c r="E90">
-        <v>40262</v>
-      </c>
-      <c r="F90" t="s">
-        <v>329</v>
-      </c>
-      <c r="G90" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7">
       <c r="A91" t="s">
         <v>95</v>
       </c>
       <c r="B91" t="s">
-        <v>125</v>
+        <v>110</v>
       </c>
       <c r="C91" t="s">
         <v>208</v>
@@ -3335,96 +3277,96 @@
         <v>298</v>
       </c>
       <c r="E91">
-        <v>126137</v>
+        <v>40262</v>
       </c>
       <c r="F91" t="s">
-        <v>308</v>
+        <v>330</v>
       </c>
       <c r="G91" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7">
       <c r="A92" t="s">
         <v>96</v>
       </c>
       <c r="B92" t="s">
-        <v>104</v>
+        <v>126</v>
       </c>
       <c r="C92" t="s">
-        <v>195</v>
+        <v>209</v>
       </c>
       <c r="D92" t="s">
         <v>299</v>
       </c>
       <c r="E92">
-        <v>16767</v>
-      </c>
-    </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
+        <v>126137</v>
+      </c>
+      <c r="F92" t="s">
+        <v>309</v>
+      </c>
+      <c r="G92" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7">
       <c r="A93" t="s">
         <v>97</v>
       </c>
       <c r="B93" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="C93" t="s">
-        <v>209</v>
+        <v>196</v>
       </c>
       <c r="D93" t="s">
         <v>300</v>
       </c>
       <c r="E93">
-        <v>33872</v>
-      </c>
-      <c r="F93" t="s">
-        <v>330</v>
-      </c>
-      <c r="G93" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
+        <v>16767</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7">
       <c r="A94" t="s">
         <v>98</v>
       </c>
       <c r="B94" t="s">
-        <v>101</v>
+        <v>110</v>
       </c>
       <c r="C94" t="s">
-        <v>124</v>
+        <v>210</v>
       </c>
       <c r="D94" t="s">
         <v>301</v>
       </c>
       <c r="E94">
-        <v>26342</v>
-      </c>
-    </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
+        <v>33872</v>
+      </c>
+      <c r="F94" t="s">
+        <v>331</v>
+      </c>
+      <c r="G94" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7">
       <c r="A95" t="s">
         <v>99</v>
       </c>
       <c r="B95" t="s">
-        <v>115</v>
+        <v>102</v>
       </c>
       <c r="C95" t="s">
-        <v>210</v>
+        <v>125</v>
       </c>
       <c r="D95" t="s">
         <v>302</v>
       </c>
       <c r="E95">
-        <v>211605</v>
-      </c>
-      <c r="F95" t="s">
-        <v>307</v>
-      </c>
-      <c r="G95" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
+        <v>26342</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7">
       <c r="A96" t="s">
         <v>100</v>
       </c>
@@ -3438,13 +3380,36 @@
         <v>303</v>
       </c>
       <c r="E96">
+        <v>211605</v>
+      </c>
+      <c r="F96" t="s">
+        <v>308</v>
+      </c>
+      <c r="G96" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="97" spans="1:7">
+      <c r="A97" t="s">
+        <v>101</v>
+      </c>
+      <c r="B97" t="s">
+        <v>117</v>
+      </c>
+      <c r="C97" t="s">
+        <v>212</v>
+      </c>
+      <c r="D97" t="s">
+        <v>304</v>
+      </c>
+      <c r="E97">
         <v>128536</v>
       </c>
-      <c r="F96" t="s">
-        <v>307</v>
-      </c>
-      <c r="G96" t="s">
-        <v>331</v>
+      <c r="F97" t="s">
+        <v>308</v>
+      </c>
+      <c r="G97" t="s">
+        <v>332</v>
       </c>
     </row>
   </sheetData>

</xml_diff>